<commit_message>
Updating IEPD after recent set of questions regarding the data model.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Search_Results/artifacts/service_model/information_model/IEPD/documentation/osbi-mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Search_Results/artifacts/service_model/information_model/IEPD/documentation/osbi-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jim/git/OJB/main/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Search_Results/artifacts/service_model/information_model/IEPD/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{96FA7C7B-E471-064C-8A5B-B0B2846C658C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EEFE8A8D-53F6-B74E-A127-15C4C65F4D48}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="860" windowWidth="32340" windowHeight="17040" xr2:uid="{66436120-2B3D-1246-B5B4-D444AC8F2095}"/>
+    <workbookView xWindow="34480" yWindow="1800" windowWidth="28800" windowHeight="17040" xr2:uid="{66436120-2B3D-1246-B5B4-D444AC8F2095}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipal Court" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="209">
   <si>
     <t>ARREST</t>
   </si>
@@ -658,6 +658,12 @@
   </si>
   <si>
     <t>Populate and Modifiable ?</t>
+  </si>
+  <si>
+    <t>NEED DB ELEMENT</t>
+  </si>
+  <si>
+    <t>USE LAST, FIRST</t>
   </si>
 </sst>
 </file>
@@ -760,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -849,10 +855,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1171,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC4E4D8-A514-1A4E-9E23-373DB4843948}">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1247,7 +1256,7 @@
       <c r="D4" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>109</v>
       </c>
       <c r="F4" s="17" t="s">
@@ -1649,8 +1658,16 @@
       <c r="B37" s="10" t="s">
         <v>152</v>
       </c>
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="E37" s="13"/>
-      <c r="F37" s="17"/>
+      <c r="F37" s="32" t="s">
+        <v>208</v>
+      </c>
       <c r="G37" s="3" t="s">
         <v>183</v>
       </c>
@@ -1659,8 +1676,16 @@
       <c r="B38" s="10" t="s">
         <v>153</v>
       </c>
+      <c r="C38" s="10">
+        <v>0</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>128</v>
+      </c>
       <c r="E38" s="13"/>
-      <c r="F38" s="17"/>
+      <c r="F38" s="32" t="s">
+        <v>207</v>
+      </c>
       <c r="G38" s="3" t="s">
         <v>154</v>
       </c>
@@ -2307,55 +2332,55 @@
       <c r="A106" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B106" s="30" t="s">
+      <c r="B106" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="C106" s="30"/>
-      <c r="D106" s="30"/>
-      <c r="E106" s="30"/>
-      <c r="F106" s="30"/>
+      <c r="C106" s="31"/>
+      <c r="D106" s="31"/>
+      <c r="E106" s="31"/>
+      <c r="F106" s="31"/>
     </row>
     <row r="107" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="B107" s="30" t="s">
+      <c r="B107" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="C107" s="30"/>
-      <c r="D107" s="30"/>
-      <c r="E107" s="30"/>
-      <c r="F107" s="30"/>
+      <c r="C107" s="31"/>
+      <c r="D107" s="31"/>
+      <c r="E107" s="31"/>
+      <c r="F107" s="31"/>
     </row>
     <row r="108" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="30" t="s">
+      <c r="A108" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="B108" s="30"/>
-      <c r="C108" s="30"/>
-      <c r="D108" s="30"/>
-      <c r="E108" s="30"/>
-      <c r="F108" s="30"/>
+      <c r="B108" s="31"/>
+      <c r="C108" s="31"/>
+      <c r="D108" s="31"/>
+      <c r="E108" s="31"/>
+      <c r="F108" s="31"/>
     </row>
     <row r="110" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="30" t="s">
+      <c r="A110" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B110" s="30"/>
-      <c r="C110" s="30"/>
-      <c r="D110" s="30"/>
-      <c r="E110" s="30"/>
-      <c r="F110" s="30"/>
+      <c r="B110" s="31"/>
+      <c r="C110" s="31"/>
+      <c r="D110" s="31"/>
+      <c r="E110" s="31"/>
+      <c r="F110" s="31"/>
     </row>
     <row r="112" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="30" t="s">
+      <c r="A112" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="B112" s="30"/>
-      <c r="C112" s="30"/>
-      <c r="D112" s="30"/>
-      <c r="E112" s="30"/>
-      <c r="F112" s="30"/>
+      <c r="B112" s="31"/>
+      <c r="C112" s="31"/>
+      <c r="D112" s="31"/>
+      <c r="E112" s="31"/>
+      <c r="F112" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
OSBI Oracle DB mapping spreadsheet update.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Search_Results/artifacts/service_model/information_model/IEPD/documentation/osbi-mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Search_Results/artifacts/service_model/information_model/IEPD/documentation/osbi-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jim/git/OJB/main/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Search_Results/artifacts/service_model/information_model/IEPD/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EEFE8A8D-53F6-B74E-A127-15C4C65F4D48}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6AA1B590-8912-0D4E-9F09-A4F56921F922}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34480" yWindow="1800" windowWidth="28800" windowHeight="17040" xr2:uid="{66436120-2B3D-1246-B5B4-D444AC8F2095}"/>
+    <workbookView xWindow="540" yWindow="1160" windowWidth="28800" windowHeight="17040" xr2:uid="{66436120-2B3D-1246-B5B4-D444AC8F2095}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipal Court" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="241">
   <si>
     <t>ARREST</t>
   </si>
@@ -449,9 +449,6 @@
     <t>Disposition</t>
   </si>
   <si>
-    <t>DISPOSITION_TYPE: Long Name</t>
-  </si>
-  <si>
     <t>What are the values for "FELONY_MISDEMEANOR" in the DB?  (currently all null)</t>
   </si>
   <si>
@@ -498,9 +495,6 @@
   </si>
   <si>
     <t>Update SENTENCE_DATE on spreadsheet</t>
-  </si>
-  <si>
-    <t>Charge at Disposition?</t>
   </si>
   <si>
     <t>NIEM</t>
@@ -615,15 +609,6 @@
     <t>ARREST.SEX</t>
   </si>
   <si>
-    <t>Charge at Arrest?</t>
-  </si>
-  <si>
-    <t>General Offense</t>
-  </si>
-  <si>
-    <t>...OFFENSE_TYPE.LONG_NAME</t>
-  </si>
-  <si>
     <t>At the request of the municipal court clerks we spoke to, we will be making this field available to them.  We will establish  a list of possible “reasons.”  This will be a dropdown where we will need to be able to control the values.</t>
   </si>
   <si>
@@ -664,6 +649,117 @@
   </si>
   <si>
     <t>USE LAST, FIRST</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>1 or 2</t>
+  </si>
+  <si>
+    <t>CHARGE.GENERAL_OFFENSE_TYPE_ID</t>
+  </si>
+  <si>
+    <t>21,14,18</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>OJBC NIEM Mapping</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/nc:Case/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Subject/nc:RoleOfPerson/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Subject/nc:RoleOfPerson/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Subject/nc:RoleOfPerson/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Subject/nc:RoleOfPerson/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Subject/nc:RoleOfPerson/j:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Subject/nc:RoleOfPerson/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Subject/nc:RoleOfPerson/nc:PersonSSNIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Subject/j:SubjectIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/nc:Disposition/nc:DispositionDate/nc:Date</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/nc:Disposition/nc:DispositionReasonText</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/nc:Disposition/chsres-ext:ConvictionCategory/chsres-ext:CategoryShortName</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/nc:Disposition/chsres-ext:DispositionCategory/chsres-ext:CategoryLongName</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/nc:Disposition/chsres-ext:DispositionFiledDate/nc:Date</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/nc:Disposition/chsres-ext:DispositionCharge/chsres-ext:ChargeCategory/chsres-ext:CategoryLongName</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Sentence/j:SentenceDeferredTerm/j:TermDuration</t>
+  </si>
+  <si>
+    <t>See above</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Sentence/j:SentenceSuspendedTerm/j:TermDuration</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Sentence/j:CourtCostAmount/nc:Amount</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Restitution/nc:ObligationDueAmount/nc:Amount</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Restitution/j:ObligationAugmentation/j:ObligationSuspendedAmount/nc:Amount</t>
+  </si>
+  <si>
+    <t>CHARGE.CHARGE_TYPE_ID/CHARGETYPE.LONG_NAME</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Charge/chsres-ext:ChargeCategory/chsres-ext:CategoryLongName</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Charge/chsres-ext:GeneralOffenseCategoryIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Arrest/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Arrest/chsres-ext:ActionCodeText</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Arrest/chsres-ext:RecordCategoryIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/nc:Case/j:CaseAugmentation/j:CaseCourt/j:OrganizationAugmentation/j:OrganizationORIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>CHARGE.FELONY_MISDEMEANOR/FELONY_MISD_TYPE/LONG_NAME</t>
+  </si>
+  <si>
+    <t>chsres-doc:CriminalHistorySearchResults/chsres-ext:CriminalHistorySearchResult/j:Charge/chsres-ext:FelonyMisdemeanorCategory/chsres-ext:CategoryLongName</t>
   </si>
 </sst>
 </file>
@@ -710,7 +806,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -732,12 +828,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -804,13 +894,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -821,15 +905,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -849,19 +924,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1178,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC4E4D8-A514-1A4E-9E23-373DB4843948}">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1191,32 +1269,39 @@
     <col min="3" max="3" width="8.5" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="10" customWidth="1"/>
     <col min="5" max="5" width="44" style="7" customWidth="1"/>
-    <col min="6" max="6" width="70" style="7" customWidth="1"/>
+    <col min="6" max="6" width="71.5" style="7" customWidth="1"/>
     <col min="7" max="7" width="74.6640625" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="10"/>
+    <col min="8" max="8" width="112" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>90</v>
       </c>
+      <c r="C1" s="8" t="s">
+        <v>204</v>
+      </c>
       <c r="D1" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>162</v>
+      <c r="F1" s="20" t="s">
+        <v>160</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>39</v>
       </c>
@@ -1229,50 +1314,56 @@
       <c r="E2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>34</v>
       </c>
+      <c r="C3" s="10" t="s">
+        <v>205</v>
+      </c>
       <c r="D3" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="240" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="C4" s="10">
         <v>0</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>164</v>
+      <c r="F4" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="27"/>
-    </row>
-    <row r="6" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="C6" s="10">
         <v>0</v>
       </c>
@@ -1282,379 +1373,443 @@
       <c r="E6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D7" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C8" s="10">
-        <v>0</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="F8" s="17" t="s">
+      <c r="H8" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C9" s="10">
-        <v>0</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="C10" s="10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="H10" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C11" s="10">
-        <v>0</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="H11" s="10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C12" s="10">
-        <v>0</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="G12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C13" s="10">
-        <v>0</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="H13" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="10">
-        <v>0</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="H14" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D15" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D16" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C15" s="10">
-        <v>0</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="17" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D16" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D17" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C18" s="10">
-        <v>0</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="17" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C19" s="10">
-        <v>0</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="17" t="s">
+      <c r="H19" s="10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="15" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="10">
-        <v>0</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="10">
-        <v>0</v>
-      </c>
+      <c r="H20" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D21" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D22" s="10" t="s">
         <v>130</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D23" s="10" t="s">
         <v>130</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" s="17"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="F23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D24" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E25" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="21"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C26" s="10">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D25" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E26" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="26"/>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C27" s="10">
-        <v>0</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="E26" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E28" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E29" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E30" s="9"/>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="15"/>
+    </row>
+    <row r="32" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="10">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="17" t="s">
+      <c r="E32" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E28" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E29" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" s="26"/>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E30" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="26"/>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E31" s="9"/>
-      <c r="F31" s="26"/>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="F32" s="17"/>
-    </row>
-    <row r="33" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="10">
-        <v>0</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="H33" s="10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C34" s="10">
+        <v>0</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" s="17" t="s">
+      <c r="E34" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="10">
-        <v>0</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="17" t="s">
+      <c r="G34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="10">
-        <v>0</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F35" s="17" t="s">
+      <c r="H35" s="10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="28"/>
+      <c r="F36" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="10">
-        <v>0</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" s="10" t="s">
         <v>152</v>
       </c>
@@ -1664,731 +1819,753 @@
       <c r="D37" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="32" t="s">
+      <c r="E37" s="28"/>
+      <c r="F37" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="10">
+        <v>0</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="15"/>
+      <c r="G39" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="15"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="10">
+        <v>0</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="15"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="10">
+        <v>0</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="10">
+        <v>0</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="10">
+        <v>0</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="10">
+        <v>0</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F49" s="15"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="15"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51" s="15"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B52" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="15"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F53" s="21"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C54" s="10">
+        <v>0</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E54" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D55" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F55" s="21"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C56" s="10">
+        <v>0</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C38" s="10">
-        <v>0</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E38" s="13"/>
-      <c r="F38" s="32" t="s">
-        <v>207</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="10">
-        <v>0</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="10">
-        <v>0</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E41" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" s="17"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B43" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="10">
-        <v>0</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B44" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="10">
-        <v>0</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B45" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" s="17"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B46" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="10">
-        <v>0</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B47" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="10">
-        <v>0</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B48" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="10">
-        <v>0</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="10">
-        <v>0</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F50" s="17"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F51" s="17"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="10" t="s">
+      <c r="H56" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D57" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E58" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" s="22"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E59" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" s="22"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E60" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="22"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E61" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F61" s="22"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F62" s="21"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C63" s="10">
+        <v>0</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E63" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D64" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" s="15"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D65" s="7"/>
+      <c r="E65" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F65" s="22"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D66" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F66" s="21"/>
+      <c r="G66" s="4"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D67" s="7"/>
+      <c r="F67" s="15"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" s="15"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F52" s="17"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F53" s="17"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F54" s="26"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C55" s="10">
-        <v>0</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="F55" s="26"/>
-      <c r="G55" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D56" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="F56" s="26"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C57" s="10">
-        <v>0</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E57" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F57" s="17"/>
-      <c r="G57" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D58" s="10" t="s">
+      <c r="D69" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F69" s="15"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F70" s="15"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F71" s="15"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D72" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F72" s="15"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E58" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F58" s="17"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E59" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="27"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E60" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F60" s="27"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E61" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F61" s="27"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E62" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F62" s="27"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B63" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F63" s="26"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C64" s="10">
-        <v>0</v>
-      </c>
-      <c r="D64" s="14" t="s">
+      <c r="E73" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F73" s="15"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F74" s="15"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D75" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E64" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F64" s="17" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D65" s="7" t="s">
+      <c r="E75" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F75" s="15"/>
+      <c r="G75" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D76" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E65" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F65" s="17"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D66" s="7"/>
-      <c r="E66" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F66" s="27"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D67" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="F67" s="26"/>
-      <c r="G67" s="4"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D68" s="7"/>
-      <c r="F68" s="17"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F69" s="17"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F70" s="17"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F71" s="17"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F72" s="17"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D73" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F73" s="17"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F74" s="17"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F75" s="17"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D76" s="14" t="s">
-        <v>130</v>
-      </c>
       <c r="E76" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F76" s="17"/>
-      <c r="G76" s="3" t="s">
-        <v>131</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="F76" s="15"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D77" s="7" t="s">
         <v>130</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F77" s="17"/>
+        <v>123</v>
+      </c>
+      <c r="F77" s="15"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D78" s="7" t="s">
-        <v>130</v>
-      </c>
+      <c r="D78" s="15"/>
       <c r="E78" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F78" s="17"/>
+        <v>124</v>
+      </c>
+      <c r="F78" s="15"/>
+      <c r="G78" s="3" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D79" s="17"/>
+      <c r="D79" s="15"/>
       <c r="E79" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F79" s="17"/>
+        <v>125</v>
+      </c>
+      <c r="F79" s="15"/>
       <c r="G79" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D80" s="17"/>
+      <c r="D80" s="13"/>
       <c r="E80" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F80" s="17"/>
+        <v>37</v>
+      </c>
+      <c r="F80" s="15"/>
       <c r="G80" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D81" s="14"/>
-      <c r="E81" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F81" s="17"/>
-      <c r="G81" s="3" t="s">
-        <v>133</v>
-      </c>
+      <c r="A81" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="F81" s="15"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D82" s="7"/>
-      <c r="F82" s="17"/>
+      <c r="F82" s="15"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D83" s="7"/>
-      <c r="F83" s="17"/>
+        <v>67</v>
+      </c>
+      <c r="F83" s="15"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F84" s="17"/>
+        <v>66</v>
+      </c>
+      <c r="F84" s="15"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F85" s="17"/>
+        <v>65</v>
+      </c>
+      <c r="F85" s="15"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F86" s="17"/>
+        <v>64</v>
+      </c>
+      <c r="F86" s="15"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F87" s="17"/>
+        <v>63</v>
+      </c>
+      <c r="F87" s="15"/>
+      <c r="G87" s="3" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F88" s="17"/>
-      <c r="G88" s="3" t="s">
-        <v>202</v>
-      </c>
+      <c r="F88" s="15"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F89" s="17"/>
+      <c r="A89" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F89" s="15"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="10" t="s">
-        <v>45</v>
-      </c>
       <c r="E90" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F90" s="17"/>
+        <v>47</v>
+      </c>
+      <c r="F90" s="15"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E91" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F91" s="17"/>
+        <v>48</v>
+      </c>
+      <c r="F91" s="15"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E92" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F92" s="17"/>
+      <c r="E92" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F92" s="22"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E93" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F93" s="27"/>
+        <v>50</v>
+      </c>
+      <c r="F93" s="22"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E94" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F94" s="27"/>
+      <c r="E94" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F94" s="15"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E95" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F95" s="17"/>
+        <v>19</v>
+      </c>
+      <c r="F95" s="15"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E96" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F96" s="17"/>
+        <v>51</v>
+      </c>
+      <c r="F96" s="15"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E97" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F97" s="17"/>
+        <v>30</v>
+      </c>
+      <c r="F97" s="15"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E98" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F98" s="17"/>
+      <c r="E98" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F98" s="22"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E99" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F99" s="27"/>
+        <v>87</v>
+      </c>
+      <c r="F99" s="22"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E100" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F100" s="27"/>
+      <c r="A100" s="18"/>
+      <c r="B100" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F100" s="15"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="23"/>
+      <c r="A101" s="17"/>
       <c r="B101" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="19"/>
+      <c r="B102" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="F101" s="17"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="22"/>
-      <c r="B102" s="10" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="24"/>
+      <c r="A103" s="23"/>
       <c r="B103" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="28"/>
-      <c r="B104" s="10" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B105" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="C105" s="27"/>
+      <c r="D105" s="27"/>
+      <c r="E105" s="27"/>
+      <c r="F105" s="27"/>
+    </row>
+    <row r="106" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B106" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
+    </row>
+    <row r="107" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="B107" s="27"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="27"/>
+    </row>
+    <row r="109" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="B109" s="27"/>
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+    </row>
+    <row r="111" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="B106" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="C106" s="31"/>
-      <c r="D106" s="31"/>
-      <c r="E106" s="31"/>
-      <c r="F106" s="31"/>
-    </row>
-    <row r="107" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B107" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="C107" s="31"/>
-      <c r="D107" s="31"/>
-      <c r="E107" s="31"/>
-      <c r="F107" s="31"/>
-    </row>
-    <row r="108" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="B108" s="31"/>
-      <c r="C108" s="31"/>
-      <c r="D108" s="31"/>
-      <c r="E108" s="31"/>
-      <c r="F108" s="31"/>
-    </row>
-    <row r="110" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="B110" s="31"/>
-      <c r="C110" s="31"/>
-      <c r="D110" s="31"/>
-      <c r="E110" s="31"/>
-      <c r="F110" s="31"/>
-    </row>
-    <row r="112" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="B112" s="31"/>
-      <c r="C112" s="31"/>
-      <c r="D112" s="31"/>
-      <c r="E112" s="31"/>
-      <c r="F112" s="31"/>
+      <c r="B111" s="27"/>
+      <c r="C111" s="27"/>
+      <c r="D111" s="27"/>
+      <c r="E111" s="27"/>
+      <c r="F111" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A110:F110"/>
-    <mergeCell ref="A112:F112"/>
+    <mergeCell ref="A109:F109"/>
+    <mergeCell ref="A111:F111"/>
+    <mergeCell ref="B105:F105"/>
     <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="A108:F108"/>
+    <mergeCell ref="A107:F107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2626,7 +2803,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2634,7 +2811,7 @@
         <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2644,7 +2821,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
         <v>137</v>
@@ -2652,12 +2829,12 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2665,32 +2842,32 @@
         <v>139</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>